<commit_message>
WFP-2436 Amend ETL logic for additional tiers
</commit_message>
<xml_diff>
--- a/test/integration/resources/WMT_PS.xlsx
+++ b/test/integration/resources/WMT_PS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlo.veo/Documents/GitHub/wmt/wmt-worker/test/integration/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary.reid/workspace/wmt-worker/test/integration/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E025ACE9-C617-6F46-B50E-C865E78443B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6AEF52-A507-224C-B80F-DF8B5F735A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38940" yWindow="8720" windowWidth="34560" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="257">
   <si>
     <t>Trust</t>
   </si>
@@ -797,6 +797,18 @@
   </si>
   <si>
     <t>Team_Cd_Offender_Manager</t>
+  </si>
+  <si>
+    <t>All NPS East Midlands Region. GAZZA</t>
+  </si>
+  <si>
+    <t>CommTierA0_S</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -818,16 +830,19 @@
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1235,9 +1250,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP3"/>
+  <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1252,21 +1269,21 @@
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
     <col min="11" max="11" width="12.5" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
-    <col min="15" max="18" width="14.83203125" customWidth="1"/>
-    <col min="19" max="30" width="12.33203125" customWidth="1"/>
-    <col min="31" max="31" width="14.6640625" customWidth="1"/>
-    <col min="32" max="47" width="10.6640625" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" customWidth="1"/>
-    <col min="49" max="64" width="13.5" customWidth="1"/>
-    <col min="65" max="65" width="17" customWidth="1"/>
-    <col min="66" max="66" width="15.5" customWidth="1"/>
-    <col min="67" max="67" width="9.83203125" customWidth="1"/>
-    <col min="68" max="68" width="13" customWidth="1"/>
+    <col min="13" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="31" width="12.33203125" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="48" width="10.6640625" customWidth="1"/>
+    <col min="49" max="49" width="14.6640625" customWidth="1"/>
+    <col min="50" max="65" width="13.5" customWidth="1"/>
+    <col min="66" max="66" width="17" customWidth="1"/>
+    <col min="67" max="67" width="15.5" customWidth="1"/>
+    <col min="68" max="68" width="9.83203125" customWidth="1"/>
+    <col min="69" max="69" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,173 +1323,176 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>68</v>
       </c>
@@ -1483,7 +1503,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>71</v>
+        <v>253</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>72</v>
@@ -1512,7 +1532,9 @@
       <c r="M2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="N2" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1523,14 +1545,14 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="6">
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6">
         <v>1</v>
       </c>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6">
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6">
         <v>1</v>
       </c>
-      <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
       <c r="AE2" s="6"/>
@@ -1567,18 +1589,19 @@
       <c r="BJ2" s="6"/>
       <c r="BK2" s="6"/>
       <c r="BL2" s="6"/>
-      <c r="BM2" s="6">
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="6">
         <v>1</v>
       </c>
-      <c r="BN2" s="6"/>
-      <c r="BO2" s="7">
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="7">
         <v>44379.022389386599</v>
       </c>
-      <c r="BP2" s="6">
+      <c r="BQ2" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
@@ -1618,29 +1641,31 @@
       <c r="M3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="6">
+      <c r="R3" s="6"/>
+      <c r="S3" s="6">
         <v>1</v>
       </c>
-      <c r="S3" s="6"/>
       <c r="T3" s="6"/>
-      <c r="U3" s="6">
+      <c r="U3" s="6"/>
+      <c r="V3" s="6">
         <v>3</v>
       </c>
-      <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="Y3" s="6">
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6">
         <v>1</v>
       </c>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6">
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6">
         <v>1</v>
       </c>
-      <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="6"/>
@@ -1677,14 +1702,15 @@
       <c r="BJ3" s="6"/>
       <c r="BK3" s="6"/>
       <c r="BL3" s="6"/>
-      <c r="BM3" s="6">
+      <c r="BM3" s="6"/>
+      <c r="BN3" s="6">
         <v>1</v>
       </c>
-      <c r="BN3" s="6"/>
-      <c r="BO3" s="7">
+      <c r="BO3" s="6"/>
+      <c r="BP3" s="7">
         <v>44379.022389386599</v>
       </c>
-      <c r="BP3" s="6">
+      <c r="BQ3" s="6">
         <v>6</v>
       </c>
     </row>

</xml_diff>